<commit_message>
Major updates; PBET prep; melconv integration; doo sound for voice; melody_dtw scoring
Former-commit-id: 42e3835f1b2f60784f9ec1a233a02c0ec808cb24 [formerly 93063c1fcf111c407eff9cadfb61f5952cc3295d]
Former-commit-id: 99e9665f6fc9907ad63b75acc9fac2d9889418ec
Former-commit-id: e85d2e3345c6fae7b5a89c67d9fe3061d2d3676f
</commit_message>
<xml_diff>
--- a/data-raw/musicassessr_dict.xlsx
+++ b/data-raw/musicassessr_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1B2437-B2BD-D043-B742-941D3823677D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B76A3E-BE7C-7A40-B78A-D96AEF4D9DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="500" windowWidth="27640" windowHeight="16860" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="147">
   <si>
     <t>mar_can_hear</t>
   </si>
@@ -472,6 +472,9 @@
   </si>
   <si>
     <t>Sing Along With This Note</t>
+  </si>
+  <si>
+    <t>Microphone</t>
   </si>
 </sst>
 </file>
@@ -880,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="92" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:B77"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="92" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1510,6 +1513,14 @@
         <v>145</v>
       </c>
     </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>146</v>
+      </c>
+      <c r="B78" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add "Stop" to dict
Former-commit-id: b36e8d482d7b5fc2617f5f48401da47a0c9be91b [formerly 71948e8b73fa9582343972961cf6a3551c6bf254]
Former-commit-id: 3ac0912f9535775617d2c020d76f7ce6c3cd6c72
Former-commit-id: 7be5350dea2d6a21ad6d72f0bc9ccfcf2d81604d
</commit_message>
<xml_diff>
--- a/data-raw/musicassessr_dict.xlsx
+++ b/data-raw/musicassessr_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE2FFC4-D813-0941-BF36-7891B3A1E658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49D6568-07E4-2449-A617-ACDC90D907DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="500" windowWidth="27640" windowHeight="16860" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="149">
   <si>
     <t>mar_can_hear</t>
   </si>
@@ -478,6 +478,9 @@
   </si>
   <si>
     <t>de</t>
+  </si>
+  <si>
+    <t>Stop</t>
   </si>
 </sst>
 </file>
@@ -886,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="92" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="92" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1756,6 +1759,17 @@
         <v>146</v>
       </c>
     </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>148</v>
+      </c>
+      <c r="B79" t="s">
+        <v>148</v>
+      </c>
+      <c r="C79" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to fix everything for HMTM 2022 testing
</commit_message>
<xml_diff>
--- a/data-raw/musicassessr_dict.xlsx
+++ b/data-raw/musicassessr_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED46A39C-ADD2-7740-948F-B21BB5F2FAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ED5A9B-FCDD-2C41-A41E-A0E48B43F69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="1100" windowWidth="33340" windowHeight="16860" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
+    <workbookView xWindow="3780" yWindow="500" windowWidth="35580" windowHeight="17200" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="221">
   <si>
     <t>mar_can_hear</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Microphone Test</t>
   </si>
   <si>
-    <t>When you are ready to record your environment for 5 seconds, press the button below.</t>
-  </si>
-  <si>
     <t>Please try not to make a noise!</t>
   </si>
   <si>
@@ -201,15 +198,9 @@
     <t>comfortable_volume</t>
   </si>
   <si>
-    <t>The volume is comfortable</t>
-  </si>
-  <si>
     <t>microphone_calibration_button</t>
   </si>
   <si>
-    <t>I can see activity in the box.</t>
-  </si>
-  <si>
     <t>microphone_calibration_message_1</t>
   </si>
   <si>
@@ -225,9 +216,6 @@
     <t xml:space="preserve">Please make sure your microphone is plugged in (if using an external microphone). </t>
   </si>
   <si>
-    <t>Wait a few seconds. You should see a black box appear. If you see activity inside the box when you make noise, then the microphone is working. Otherwise, it is not.</t>
-  </si>
-  <si>
     <t>record_bg</t>
   </si>
   <si>
@@ -408,12 +396,6 @@
     <t>If you have any questions, please ask the researcher before proceeding.</t>
   </si>
   <si>
-    <t>Please play/sing the lowest note on your instrument/voice. Press Stop when you are finished.</t>
-  </si>
-  <si>
-    <t>Please play/sing the highest note on your instrument/voice. Press Stop when you are finished.</t>
-  </si>
-  <si>
     <t>Try_Again</t>
   </si>
   <si>
@@ -468,18 +450,12 @@
     <t>Stop</t>
   </si>
   <si>
-    <t>When you are ready, click on the microphone image. If you see a popup message that says “Allow”,  click “Allow”.</t>
-  </si>
-  <si>
     <t>We need to record 5 seconds of the background sound level of the room while you are quiet.</t>
   </si>
   <si>
     <t>When you are ready to record the background sound level, press the button below.</t>
   </si>
   <si>
-    <t>Vocal Signal Sound Level Test</t>
-  </si>
-  <si>
     <t>When you are ready, click on “Record” and for about 5 seconds please hum, directed toward your microphone for 5 seconds.  (to “hum”, put your lips together and make a sound with your voice.)</t>
   </si>
   <si>
@@ -489,12 +465,6 @@
     <t>The test will not work in Safari or Internet Explorer and potentially other browsers.</t>
   </si>
   <si>
-    <t>Please play/sing the lowest comfortable note on your instrument/voice. Press Stop when you are finished.</t>
-  </si>
-  <si>
-    <t>Please play/sing the highest comfortable  note on your instrument/voice. Press Stop when you are finished.</t>
-  </si>
-  <si>
     <t>other_please_state</t>
   </si>
   <si>
@@ -529,13 +499,211 @@
   </si>
   <si>
     <t>Bitte wählen Sie, welches Instrument Sie benuzten werden.</t>
+  </si>
+  <si>
+    <t>select_midi_device_title</t>
+  </si>
+  <si>
+    <t>Select MIDI device</t>
+  </si>
+  <si>
+    <t>MIDI-Gerät auswählen.</t>
+  </si>
+  <si>
+    <t>select_midi_device_message</t>
+  </si>
+  <si>
+    <t>Your device should have been plugged in before you reached this page. It may take a moment to appear.</t>
+  </si>
+  <si>
+    <t>Ihr Gerät sollte bereits angeschlossen gewesen sein bevor Sie diese Seite erreichen haben. Es kann einen Moment dauern bis es erscheint.</t>
+  </si>
+  <si>
+    <t>no_midi_device_found</t>
+  </si>
+  <si>
+    <t>No MIDI device found.</t>
+  </si>
+  <si>
+    <t>Kein MIDI-Gerät gefunden.</t>
+  </si>
+  <si>
+    <t>range_explanation_voice</t>
+  </si>
+  <si>
+    <t>We will now find your approximate voice range. You will be asked first to sing your lowest comfortable note.  The computer will then analyse this note and it will be played back to you. You will be asked to decide if this is a good match to your lowest note. Sometimes the computer can make a large error. You should know when that happens, and you will have an opportunity to sing your  note again, and give the computer another chance.</t>
+  </si>
+  <si>
+    <t>range_explanation_instrument</t>
+  </si>
+  <si>
+    <t>We will now find your approximate instrument range. You will be asked to play your lowest comfortable note, then highest comfortable note.</t>
+  </si>
+  <si>
+    <t>get_range_low</t>
+  </si>
+  <si>
+    <t>get_range_low_note_voice</t>
+  </si>
+  <si>
+    <t>get_range_high_note_voice</t>
+  </si>
+  <si>
+    <t>Please play the lowest comfortable note on your instrument. Press Stop when you are finished.</t>
+  </si>
+  <si>
+    <t>Please play the highest comfortable  note on your instrument. Press Stop when you are finished.</t>
+  </si>
+  <si>
+    <t>Please sing your lowest comfortable note. Press Stop when you are finished.</t>
+  </si>
+  <si>
+    <t>Please sing your highest comfortable note. Press Stop when you are finished.</t>
+  </si>
+  <si>
+    <t>audio_error_suggestion</t>
+  </si>
+  <si>
+    <t>Perhaps you are too quiet, or you have a noisy computer fan.</t>
+  </si>
+  <si>
+    <t>hear_range</t>
+  </si>
+  <si>
+    <t>range_adjust_message</t>
+  </si>
+  <si>
+    <t>You can click below to hear your range.</t>
+  </si>
+  <si>
+    <t>Please note, we may have changed the range to be slightly higher or lower than you actually sang.</t>
+  </si>
+  <si>
+    <t>sing_hbd</t>
+  </si>
+  <si>
+    <t>Please sing Happy Birthday.</t>
+  </si>
+  <si>
+    <t>Please note, we may have changed the range to be slightly higher or lower than you actually played.</t>
+  </si>
+  <si>
+    <t>range_adjust_message_voice</t>
+  </si>
+  <si>
+    <t>first_note_is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The first note is: </t>
+  </si>
+  <si>
+    <t>play_first_note</t>
+  </si>
+  <si>
+    <t>Play First Note</t>
+  </si>
+  <si>
+    <t>transposed</t>
+  </si>
+  <si>
+    <t>Please note, this is transposed for your instrument.</t>
+  </si>
+  <si>
+    <t>Make a sound (e.g., hum, clap, sing).  If you see activity  (moving coloured lines) inside the meter when you make a sound, then the microphone is working. Otherwise, it is not.</t>
+  </si>
+  <si>
+    <t>I can see activity on the meter.</t>
+  </si>
+  <si>
+    <t>long_tone_text</t>
+  </si>
+  <si>
+    <t>Sing along with the tone for 5 seconds.</t>
+  </si>
+  <si>
+    <t>you_have_completed_the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have completed the </t>
+  </si>
+  <si>
+    <t>Click to proceed to the next test.</t>
+  </si>
+  <si>
+    <t>proceed_next_test</t>
+  </si>
+  <si>
+    <t>Ich kann die Musik hören, bitte fortfahren.</t>
+  </si>
+  <si>
+    <t>Kopfhörertest</t>
+  </si>
+  <si>
+    <t>Sie sollten jetzt Audio spielen hören.</t>
+  </si>
+  <si>
+    <t>Bitte passen Sie die Kopfhörerlautstärke auf ein komfortables Level an.</t>
+  </si>
+  <si>
+    <t>Wenn es Ihnen nicht möglich ist die Kopfhörerlautstärke auf ein komfortables Level anzupassen, fahren Sie bitte nicht fort.</t>
+  </si>
+  <si>
+    <t>Die Lautstärke ist angenehm.</t>
+  </si>
+  <si>
+    <t>The volume is comfortable.</t>
+  </si>
+  <si>
+    <t>Mikrofontest</t>
+  </si>
+  <si>
+    <t>Bitte stellen Sie sicher, dass Ihr Mikrofon angeschlossen ist (wenn Sie ein externes Mikrofon benutzten).</t>
+  </si>
+  <si>
+    <t>Klicken Sie auf den "Start test" Knopf. Wenn die Nachricht "Zulassen" erscheint, klicken Sie "Zulassen".</t>
+  </si>
+  <si>
+    <t>Click on the "Start test" button. If you see a popup message that says "Allow", click "Allow".</t>
+  </si>
+  <si>
+    <t>Machen Sie ein Geräusch (z.B. summen, klatschen, singen). Wenn Sie, während Sie das Geräusch machen, innerhalb des Geräuschpegelfensters Bewegung sehen (farbige Linien die sich bewegen), dann funktioniert das Mikrofon. Andernfalls funktioniert es nicht.</t>
+  </si>
+  <si>
+    <t>Signal Volume Test</t>
+  </si>
+  <si>
+    <t>Signalvolumentest</t>
+  </si>
+  <si>
+    <t>Auf der nächsten Seite testen wie ob ihr Hintergrund zu laut war oder nicht. Wenn Ihr Hintergrund zu laut ist, können Sie den Test leider nicht durchführen. Es kann einige Sekunden dauern, die Seite zu laden.</t>
+  </si>
+  <si>
+    <t>Wir müssen jetzt 5 Sekunden des Hintergrundgeräuschpegels in ihrem Raum aufnehmen während Sie sich still verhalten.</t>
+  </si>
+  <si>
+    <t>Wenn Sie bereit sind, Ihre Hintergrundgeräusche für 5 Sekunden aufzunehmen, drücken Sie den Knopf unten.</t>
+  </si>
+  <si>
+    <t>Bitte versuchen Sie keine Geräusche zu machen!</t>
+  </si>
+  <si>
+    <t>Ich Bin Bereit Meine Hintergrundgeräusche Aufzunehmen</t>
+  </si>
+  <si>
+    <t>Weiter</t>
+  </si>
+  <si>
+    <t>Setup Bereit</t>
+  </si>
+  <si>
+    <t>Okay, jetzt ist alles eingestellt. Klick um zu den Hauptaufgaben fortzufahren.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -580,15 +748,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -599,6 +760,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -614,15 +781,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -630,9 +794,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -947,27 +1120,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="92" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.6640625" customWidth="1"/>
     <col min="2" max="2" width="155.5" customWidth="1"/>
+    <col min="3" max="3" width="175.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -978,898 +1152,1107 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>205</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>144</v>
+        <v>209</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>144</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>63</v>
+        <v>191</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>63</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>57</v>
+        <v>192</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>147</v>
+        <v>64</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>70</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>145</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>8</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>10</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>12</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="306" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="15" customFormat="1" ht="306" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>18</v>
+      <c r="C22" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C28" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="C30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C31" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C36" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="C37" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C42" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B48" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="C48" t="s">
-        <v>124</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B49" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="C49" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>88</v>
+      <c r="A50" t="s">
+        <v>169</v>
+      </c>
+      <c r="B50" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>170</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" t="s">
-        <v>90</v>
-      </c>
-      <c r="C52" t="s">
-        <v>90</v>
+      <c r="A52" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>91</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>107</v>
+        <v>85</v>
+      </c>
+      <c r="B53" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>106</v>
+        <v>86</v>
+      </c>
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>93</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>108</v>
+        <v>87</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>94</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>104</v>
+        <v>88</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>95</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>105</v>
+        <v>89</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>157</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>158</v>
+        <v>90</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>159</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>160</v>
+        <v>91</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>99</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>100</v>
+        <v>149</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>101</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>102</v>
+        <v>93</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="7" t="s">
+      <c r="A63" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="C63" s="7" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>109</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>110</v>
+        <v>97</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>113</v>
+      <c r="A65" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>112</v>
+      <c r="A66" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>119</v>
+      <c r="B68" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" t="s">
+        <v>114</v>
+      </c>
+      <c r="C71" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C72" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C69" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
+      <c r="B73" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>120</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B74" t="s">
         <v>121</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C74" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>126</v>
-      </c>
-      <c r="B72" t="s">
-        <v>127</v>
-      </c>
-      <c r="C72" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>128</v>
-      </c>
-      <c r="B73" t="s">
-        <v>128</v>
-      </c>
-      <c r="C73" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B75" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C75" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>133</v>
+      <c r="A76" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B77" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C77" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>138</v>
-      </c>
-      <c r="B78" t="s">
-        <v>137</v>
-      </c>
-      <c r="C78" t="s">
-        <v>137</v>
+      <c r="A78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>140</v>
+      <c r="A79" t="s">
+        <v>129</v>
+      </c>
+      <c r="B79" t="s">
+        <v>168</v>
+      </c>
+      <c r="C79" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B80" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C80" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>143</v>
-      </c>
-      <c r="B81" t="s">
-        <v>143</v>
-      </c>
-      <c r="C81" t="s">
-        <v>143</v>
+      <c r="A81" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>153</v>
-      </c>
-      <c r="B82" t="s">
-        <v>154</v>
-      </c>
-      <c r="C82" t="s">
-        <v>154</v>
+      <c r="A82" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>135</v>
+      </c>
+      <c r="B83" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>137</v>
+      </c>
+      <c r="B84" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>143</v>
+      </c>
+      <c r="B85" t="s">
+        <v>144</v>
+      </c>
+      <c r="C85" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86" t="s">
+        <v>146</v>
+      </c>
+      <c r="C86" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B87" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C87" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>164</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>166</v>
+      </c>
+      <c r="B91" t="s">
+        <v>167</v>
+      </c>
+      <c r="C91" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>175</v>
+      </c>
+      <c r="B92" t="s">
+        <v>176</v>
+      </c>
+      <c r="C92" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>177</v>
+      </c>
+      <c r="B93" t="s">
+        <v>179</v>
+      </c>
+      <c r="C93" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>184</v>
+      </c>
+      <c r="B94" t="s">
+        <v>180</v>
+      </c>
+      <c r="C94" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>178</v>
+      </c>
+      <c r="B95" t="s">
+        <v>183</v>
+      </c>
+      <c r="C95" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>181</v>
+      </c>
+      <c r="B96" t="s">
+        <v>182</v>
+      </c>
+      <c r="C96" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>185</v>
+      </c>
+      <c r="B97" t="s">
+        <v>186</v>
+      </c>
+      <c r="C97" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>187</v>
+      </c>
+      <c r="B98" t="s">
+        <v>188</v>
+      </c>
+      <c r="C98" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>189</v>
+      </c>
+      <c r="B99" t="s">
+        <v>190</v>
+      </c>
+      <c r="C99" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>86</v>
+      </c>
+      <c r="B100" t="s">
+        <v>86</v>
+      </c>
+      <c r="C100" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>195</v>
+      </c>
+      <c r="B101" t="s">
+        <v>196</v>
+      </c>
+      <c r="C101" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>198</v>
+      </c>
+      <c r="B102" t="s">
+        <v>197</v>
+      </c>
+      <c r="C102" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make sure max_goes trickles to record_ui
</commit_message>
<xml_diff>
--- a/data-raw/musicassessr_dict.xlsx
+++ b/data-raw/musicassessr_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EB01DE-0EC7-E145-8E0E-DF8881691006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847623A8-A323-4E4D-97F0-49EEC649CCBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19620" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
   </bookViews>
@@ -411,9 +411,6 @@
     <t>Range_Test</t>
   </si>
   <si>
-    <t>Copy the melody you hear</t>
-  </si>
-  <si>
     <t>copy_melody_title</t>
   </si>
   <si>
@@ -801,18 +798,9 @@
     <t>Wenn Sie noch Fragen haben, wenden Sie sich bitte an den Forscher bevor Sie weitermachen.</t>
   </si>
   <si>
-    <t>Nochmal versuchen</t>
-  </si>
-  <si>
     <t>Weitermachen</t>
   </si>
   <si>
-    <t>Wenn Sie mit Ihren Antworten zufrieden waren, klicken Sie auf "weiter", andernfalls klicken Sie "nochmal versuchen".</t>
-  </si>
-  <si>
-    <t>If you were happy with your response, please click to "continue", otherwise please click to "try again".</t>
-  </si>
-  <si>
     <t>Browservorraussetzungen</t>
   </si>
   <si>
@@ -931,6 +919,18 @@
   </si>
   <si>
     <t>Range Test</t>
+  </si>
+  <si>
+    <t>If you were happy with your response, please click to "Continue", otherwise please click to "Try Again".</t>
+  </si>
+  <si>
+    <t>Wenn Sie mit Ihren Antworten zufrieden waren, klicken Sie auf "Weiter", andernfalls klicken Sie "Nochmal Versuchen".</t>
+  </si>
+  <si>
+    <t>Nochmal Versuchen</t>
+  </si>
+  <si>
+    <t>Copy The Melody You Hear</t>
   </si>
 </sst>
 </file>
@@ -1423,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}">
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1442,7 +1442,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1453,7 +1453,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1464,7 +1464,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1472,10 +1472,10 @@
         <v>48</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1483,10 +1483,10 @@
         <v>49</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1497,18 +1497,18 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1516,10 +1516,10 @@
         <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1530,18 +1530,18 @@
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1552,7 +1552,7 @@
         <v>57</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1560,10 +1560,10 @@
         <v>54</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1571,10 +1571,10 @@
         <v>56</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1582,10 +1582,10 @@
         <v>52</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1593,10 +1593,10 @@
         <v>62</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1607,7 +1607,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1615,10 +1615,10 @@
         <v>58</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1626,10 +1626,10 @@
         <v>59</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1640,7 +1640,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1651,7 +1651,7 @@
         <v>6</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1662,7 +1662,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1673,7 +1673,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -1684,7 +1684,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1695,7 +1695,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1747,10 +1747,10 @@
         <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1761,7 +1761,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1772,7 +1772,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1783,7 +1783,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1794,7 +1794,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1805,7 +1805,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1813,10 +1813,10 @@
         <v>35</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1827,7 +1827,7 @@
         <v>76</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1838,7 +1838,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1849,7 +1849,7 @@
         <v>39</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1860,7 +1860,7 @@
         <v>41</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1871,7 +1871,7 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1882,7 +1882,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1893,7 +1893,7 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1912,10 +1912,10 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1926,7 +1926,7 @@
         <v>67</v>
       </c>
       <c r="C45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1937,7 +1937,7 @@
         <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1948,7 +1948,7 @@
         <v>71</v>
       </c>
       <c r="C47" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1959,7 +1959,7 @@
         <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1967,10 +1967,10 @@
         <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1978,10 +1978,10 @@
         <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1989,32 +1989,32 @@
         <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2025,7 +2025,7 @@
         <v>80</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2036,7 +2036,7 @@
         <v>81</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2047,7 +2047,7 @@
         <v>82</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2058,7 +2058,7 @@
         <v>99</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2069,7 +2069,7 @@
         <v>98</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2080,7 +2080,7 @@
         <v>100</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2091,7 +2091,7 @@
         <v>96</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2102,29 +2102,29 @@
         <v>97</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="C62" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>141</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>143</v>
-      </c>
       <c r="C63" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -2135,7 +2135,7 @@
         <v>90</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2146,7 +2146,7 @@
         <v>92</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2157,7 +2157,7 @@
         <v>94</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2168,7 +2168,7 @@
         <v>95</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2179,7 +2179,7 @@
         <v>102</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -2190,7 +2190,7 @@
         <v>105</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2201,7 +2201,7 @@
         <v>104</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2212,7 +2212,7 @@
         <v>103</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -2223,7 +2223,7 @@
         <v>111</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2234,7 +2234,7 @@
         <v>110</v>
       </c>
       <c r="C73" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2245,7 +2245,7 @@
         <v>113</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2256,7 +2256,7 @@
         <v>115</v>
       </c>
       <c r="C75" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2267,7 +2267,7 @@
         <v>117</v>
       </c>
       <c r="C76" t="s">
-        <v>255</v>
+        <v>297</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2278,7 +2278,7 @@
         <v>118</v>
       </c>
       <c r="C77" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -2286,10 +2286,10 @@
         <v>119</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>258</v>
+        <v>295</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -2300,7 +2300,7 @@
         <v>120</v>
       </c>
       <c r="C79" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2311,7 +2311,7 @@
         <v>122</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2319,285 +2319,285 @@
         <v>124</v>
       </c>
       <c r="B81" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C81" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B82" t="s">
-        <v>125</v>
+        <v>298</v>
       </c>
       <c r="C82" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="C83" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="C84" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C87" s="27" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B88" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C88" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B89" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C89" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>135</v>
+      </c>
+      <c r="B90" t="s">
         <v>136</v>
       </c>
-      <c r="B90" t="s">
-        <v>137</v>
-      </c>
       <c r="C90" s="22" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>137</v>
+      </c>
+      <c r="B91" t="s">
         <v>138</v>
       </c>
-      <c r="B91" t="s">
-        <v>139</v>
-      </c>
       <c r="C91" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="C92" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B93" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B93" s="8" t="s">
-        <v>152</v>
-      </c>
       <c r="C93" s="9" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="C94" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>155</v>
+      </c>
+      <c r="B95" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B95" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="C95" s="21" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>157</v>
+      </c>
+      <c r="B96" t="s">
         <v>158</v>
       </c>
-      <c r="B96" t="s">
-        <v>159</v>
-      </c>
       <c r="C96" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>165</v>
+      </c>
+      <c r="B97" t="s">
         <v>166</v>
       </c>
-      <c r="B97" t="s">
-        <v>167</v>
-      </c>
       <c r="C97" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B98" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C98" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B99" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C99" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B100" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C100" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>171</v>
+      </c>
+      <c r="B101" t="s">
         <v>172</v>
       </c>
-      <c r="B101" t="s">
-        <v>173</v>
-      </c>
       <c r="C101" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>175</v>
+      </c>
+      <c r="B102" t="s">
         <v>176</v>
       </c>
-      <c r="B102" t="s">
-        <v>177</v>
-      </c>
       <c r="C102" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>177</v>
+      </c>
+      <c r="B103" t="s">
         <v>178</v>
       </c>
-      <c r="B103" t="s">
-        <v>179</v>
-      </c>
       <c r="C103" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>179</v>
+      </c>
+      <c r="B104" t="s">
         <v>180</v>
       </c>
-      <c r="B104" t="s">
-        <v>181</v>
-      </c>
       <c r="C104" s="22" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>184</v>
+      </c>
+      <c r="B105" t="s">
         <v>185</v>
       </c>
-      <c r="B105" t="s">
-        <v>186</v>
-      </c>
       <c r="C105" s="22" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B106" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C106" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality to support two different long tone singing paradigms: call_and_response or sing_along.
</commit_message>
<xml_diff>
--- a/data-raw/musicassessr_dict.xlsx
+++ b/data-raw/musicassessr_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE32D59-A4EE-2340-BA1F-4001A61CDA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657622C7-F8BF-104B-AF58-080D4211D9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="500" windowWidth="28800" windowHeight="17000" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
+    <workbookView xWindow="5600" yWindow="500" windowWidth="28800" windowHeight="17000" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="470">
   <si>
     <t>mar_can_hear</t>
   </si>
@@ -1423,6 +1423,30 @@
   </si>
   <si>
     <t>long_tone_title</t>
+  </si>
+  <si>
+    <t>long_tone_title_call_and_response</t>
+  </si>
+  <si>
+    <t>long_tone_text_call_and_response</t>
+  </si>
+  <si>
+    <t>long_tone_instruction_call_and_response</t>
+  </si>
+  <si>
+    <t>long_tone_instruction_call_and_response_2</t>
+  </si>
+  <si>
+    <t>long_tone_instruction_call_and_response_3</t>
+  </si>
+  <si>
+    <t>Sing Back The Note After Your Hear It</t>
+  </si>
+  <si>
+    <t>Sing back the note for 5 seconds after you hear it.</t>
+  </si>
+  <si>
+    <t>Please try and sing the exact same note and hold after you hear it.</t>
   </si>
 </sst>
 </file>
@@ -1919,15 +1943,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}">
-  <dimension ref="A1:D145"/>
+  <dimension ref="A1:D150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" topLeftCell="C128" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="1" max="1" width="57" customWidth="1"/>
     <col min="2" max="3" width="155.5" customWidth="1"/>
     <col min="4" max="4" width="175.5" customWidth="1"/>
   </cols>
@@ -3962,6 +3986,76 @@
         <v>460</v>
       </c>
     </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B150" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="C150" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="D150" s="21" t="s">
+        <v>283</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D135" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Italian translations for musicassessr pages
</commit_message>
<xml_diff>
--- a/data-raw/musicassessr_dict.xlsx
+++ b/data-raw/musicassessr_dict.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657622C7-F8BF-104B-AF58-080D4211D9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65974C08-73EA-E847-8FDC-A6EE4C02008A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="500" windowWidth="28800" windowHeight="17000" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20880" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$D$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$D$136</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="500">
   <si>
     <t>mar_can_hear</t>
   </si>
@@ -414,6 +414,9 @@
     <t>copy_melody_title</t>
   </si>
   <si>
+    <t>long_tone_heading</t>
+  </si>
+  <si>
     <t>Sing Along With This Note</t>
   </si>
   <si>
@@ -939,9 +942,6 @@
     <t>Dovresti sentire dell'audio in riproduzione. Puoi iniziare e stoppare l'audio cliccando sul triangolo.</t>
   </si>
   <si>
-    <t>Se il volume non è comodo, regolalo a un livello confortevole attraverso il tuo modo normale di cambiare il volume sul tuo computer.</t>
-  </si>
-  <si>
     <t>Se non riesci a riprodurre l'audio a un livello confortevole, non continuare.</t>
   </si>
   <si>
@@ -990,9 +990,6 @@
     <t>Continua</t>
   </si>
   <si>
-    <t>Emetti un suono (ad esempio, canticchia a bocca chiusa, batti le mani, canta). Se vedi attività (barra colorata in movimento) all'interno del misuratore quando emetti un suono, significa che il microfono funziona. Altrimenti, non sta funzionando.</t>
-  </si>
-  <si>
     <t>Installazione completata</t>
   </si>
   <si>
@@ -1185,12 +1182,6 @@
     <t>Nessun dispositivo MIDI trovato.</t>
   </si>
   <si>
-    <t>Ora troveremo l'estensione approssimativa del vostro strumento. Vi verrà chiesto di suonare la vostra nota più grave e comoda, poi quella più acuta.</t>
-  </si>
-  <si>
-    <t>Ora troveremo la vostra estensione vocale approssimativa. Per prima cosa, vi verrà chiesto di cantare la vostra nota più grave e comoda.  Il computer analizzerà questa nota e ve la riproporrà. Vi verrà chiesto di decidere se questa nota corrisponde alla vostra nota più grave. A volte il computer può commettere un grosso errore. Quando ciò accade, si deve sapere che si ha l'opportunità di cantare di nuovo la propria nota e di dare al computer un'altra possibilità.</t>
-  </si>
-  <si>
     <t>Se la nota ti sembra fuori dalla tua estensione vocale, canta il suono che corrisponde meglio alla nota nella tua estensione, ad esempio, in un'ottava diversa.</t>
   </si>
   <si>
@@ -1203,9 +1194,6 @@
     <t>È possibile che l'estensione sia stata modificata in modo da risultare leggermente più alta o più bassa di quella effettivamente cantata.</t>
   </si>
   <si>
-    <t>È possibile che la gamma sia stata modificata in modo da risultare leggermente più alta o più bassa di quella effettivamente suonata.</t>
-  </si>
-  <si>
     <t>Per favore, canta Buon Compleanno</t>
   </si>
   <si>
@@ -1221,9 +1209,6 @@
     <t>Hai completato il</t>
   </si>
   <si>
-    <t>Cicca per proseguire col prossimo test.</t>
-  </si>
-  <si>
     <t>browser_recommendation</t>
   </si>
   <si>
@@ -1248,6 +1233,9 @@
     <t>Thank you</t>
   </si>
   <si>
+    <t>Danke</t>
+  </si>
+  <si>
     <t>concise_headphone_wording</t>
   </si>
   <si>
@@ -1287,6 +1275,9 @@
     <t>Your vocal signal compared to the background noise is not sufficient for testing. Please find a quieter space, get closer to the mic, or adjust the volume and we will measure the vocal signal sound level again. If neither of these is possible for you, please email sebsilas@gmail.com with 'weak signal' in the subject space, and you will be contacted within 24 hours to troubleshoot this problem. You may also end the program and attempt to adjust your microphone volume and start the program again.</t>
   </si>
   <si>
+    <t>Not sure</t>
+  </si>
+  <si>
     <t>Your response was not understood. Perhaps your microphone is not setup correctly.</t>
   </si>
   <si>
@@ -1380,9 +1371,6 @@
     <t>were_you_happy</t>
   </si>
   <si>
-    <t>'If you were happy with your response, please click to "Continue", otherwise please click to "Try Again".'</t>
-  </si>
-  <si>
     <t>You_have</t>
   </si>
   <si>
@@ -1422,31 +1410,133 @@
     <t>Now you will hear some melodies with rhythms. Please try and sing the melodies with their rhythms.</t>
   </si>
   <si>
-    <t>long_tone_title</t>
-  </si>
-  <si>
-    <t>long_tone_title_call_and_response</t>
-  </si>
-  <si>
-    <t>long_tone_text_call_and_response</t>
-  </si>
-  <si>
-    <t>long_tone_instruction_call_and_response</t>
-  </si>
-  <si>
-    <t>long_tone_instruction_call_and_response_2</t>
-  </si>
-  <si>
-    <t>long_tone_instruction_call_and_response_3</t>
-  </si>
-  <si>
-    <t>Sing Back The Note After Your Hear It</t>
-  </si>
-  <si>
-    <t>Sing back the note for 5 seconds after you hear it.</t>
-  </si>
-  <si>
-    <t>Please try and sing the exact same note and hold after you hear it.</t>
+    <t>Se il volume non è comodo, regolalo a un livello confortevole attraverso il normale metodo di modifica del volume sul tuo computer.</t>
+  </si>
+  <si>
+    <t>Per ottenere risultati ottimali, eseguire questo test con i browser Google Chrome o Opera. Altri browser possono comunque funzionare.</t>
+  </si>
+  <si>
+    <t>Ora prepariamo il tutto.</t>
+  </si>
+  <si>
+    <t>Grazie</t>
+  </si>
+  <si>
+    <t>Per favore, assicurati che le cuffie funzionino e regola il volume a un buon livello.</t>
+  </si>
+  <si>
+    <t>Per fare questo, utilizza il normale metodo di modifica del volume sul tuo computer.</t>
+  </si>
+  <si>
+    <t>Tipo di Microfono</t>
+  </si>
+  <si>
+    <t>Interno</t>
+  </si>
+  <si>
+    <t>Stai utilizzando un microfono interno (integrato) o esterno (collegato)?</t>
+  </si>
+  <si>
+    <t>Non sono sicuro/a</t>
+  </si>
+  <si>
+    <t>Il segnale vocale rispetto al rumore di fondo non è sufficiente per il test. Si prega di trovare uno spazio più silenzioso, di avvicinarsi al microfono o di regolare il volume e di misurare nuovamente il livello del segnale vocale. Se nessuna di queste opzioni è possibile, inviate un'e-mail a sebsilas@gmail.com scrivendo "segnale debole" nell'oggetto e sarete contattati entro 24 ore per risolvere il problema. È anche possibile chiudere il programma, tentare di regolare il volume del microfono e riaprire il programma.</t>
+  </si>
+  <si>
+    <t>La risposta non è stata compresa. Forse il microfono non è impostato correttamente.</t>
+  </si>
+  <si>
+    <t>Verifica del livello di rumore di fondo</t>
+  </si>
+  <si>
+    <t>Il livello di rumore di fondo è buono</t>
+  </si>
+  <si>
+    <t>Se appare un messaggio, fare clic su Consenti. Fare clic su Avvia test per verificare se il microfono funziona. Emetti un suono.</t>
+  </si>
+  <si>
+    <t>Se l'indicatore è rosso quando suoni lo strumento, non procedere. Abbassa il volume di ingresso del microfono o allontanati da esso.</t>
+  </si>
+  <si>
+    <t>Avvia il test</t>
+  </si>
+  <si>
+    <t>Quando sei pronto/a, clicca su "Registra" e per circa 5 secondi canticchia, rivolgendoti verso microfono  (per "canticchiare", unisci le labbra ed emetti un suono con la voce).</t>
+  </si>
+  <si>
+    <t>È possibile che l'estensione sia stata modificata in modo da risultare leggermente più alta o più bassa di quella effettivamente suonata.</t>
+  </si>
+  <si>
+    <t>Ora troveremo la tua estensione vocale indicativa. Ti verrà chiesto di cantare prima la nota più grave e confortevole per la tua voce, poi quella più acuta. Ad ogni tentativo, il computer analizzerà la nota cantata. Se ritieni che non sia stata registrata la nota giusta, puoi provare di nuovo.</t>
+  </si>
+  <si>
+    <t>Istruzioni</t>
+  </si>
+  <si>
+    <t>Fai clic qui sotto per ascoltare la melodia. Canta la melodia. Clicca su Stop al termine.</t>
+  </si>
+  <si>
+    <t>Ora sentirete alcune melodie. Per favore, prova a cantare le melodie.</t>
+  </si>
+  <si>
+    <t>Registrazione audio</t>
+  </si>
+  <si>
+    <t>Clicca su "registra" per registrare l'audio</t>
+  </si>
+  <si>
+    <t>If you were happy with your response, please click to "Continue", otherwise please click to "Try Again".'</t>
+  </si>
+  <si>
+    <t>Se sei soddisfatto della tua risposta, fai clic su "Continua", altrimenti fai clic su "Riprova".</t>
+  </si>
+  <si>
+    <t>Non rimangono più tentativi. Fai clic per ascoltare la prossima melodia.</t>
+  </si>
+  <si>
+    <t>tentativi ancora a disposizione, se vuoi.</t>
+  </si>
+  <si>
+    <t>È rimasto un solo tentativo</t>
+  </si>
+  <si>
+    <t>tentativi rimanenti.</t>
+  </si>
+  <si>
+    <t>Hai un tentativo ancora a disposizione, se vuoi.</t>
+  </si>
+  <si>
+    <t>tentativi a disposizione, se vuoi.</t>
+  </si>
+  <si>
+    <t>Fai clic qui sotto per ascoltare la melodia. Canta la melodia e il ritmo. Fai clic su Stop quando hai finito.</t>
+  </si>
+  <si>
+    <t>Canta la melodia e i ritmi.</t>
+  </si>
+  <si>
+    <t>Ora ascolterai alcune melodie ritmate. Prova a cantare le melodie con il loro ritmo.</t>
+  </si>
+  <si>
+    <t>Sezione Progressi</t>
+  </si>
+  <si>
+    <t>Clicca per proseguire col prossimo test.</t>
+  </si>
+  <si>
+    <t>Fornite un identificativo anonimo che conoscete solo voi, nel caso in cui qualcosa vada storto.</t>
+  </si>
+  <si>
+    <t>Emetti un suono (ad esempio, canticchia a bocca chiusa, batti le mani, canta). Se vedi attività (barra colorata in movimento) all'interno del metro quando emetti un suono, significa che il microfono funziona. Altrimenti, non sta funzionando.</t>
+  </si>
+  <si>
+    <t>Se il metro funziona, si dovrebbero vedere i colori muoversi. In caso contrario, provare a impostare nuovamente il microfono e riprendere il test.</t>
+  </si>
+  <si>
+    <t>Ora troveremo la vostra estensione vocale indicativa. Per prima cosa, vi verrà chiesto di cantare la vostra nota più grave e comoda.  Il computer analizzerà questa nota e ve la riproporrà. Vi verrà chiesto di decidere se questa nota corrisponde alla vostra nota più grave. A volte il computer può commettere un grosso errore. Quando ciò accade, si deve sapere che si ha l'opportunità di cantare di nuovo la propria nota e di dare al computer un'altra possibilità.</t>
+  </si>
+  <si>
+    <t>Ora troveremo l'estensione indicativa del vostro strumento. Vi verrà chiesto di suonare la vostra nota più grave e comoda, poi quella più acuta.</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1629,6 +1719,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1943,16 +2034,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C128" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="91" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57" customWidth="1"/>
-    <col min="2" max="3" width="155.5" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="155.5" customWidth="1"/>
+    <col min="3" max="3" width="179.5" customWidth="1"/>
     <col min="4" max="4" width="175.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1964,10 +2056,10 @@
         <v>13</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1978,10 +2070,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1995,7 +2087,7 @@
         <v>305</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2003,13 +2095,13 @@
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2017,13 +2109,13 @@
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C5" t="s">
-        <v>300</v>
+        <v>457</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2037,21 +2129,21 @@
         <v>301</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>279</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>278</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>302</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2059,13 +2151,13 @@
         <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>303</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2079,21 +2171,21 @@
         <v>304</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>306</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2107,7 +2199,7 @@
         <v>307</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2115,13 +2207,13 @@
         <v>54</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>308</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2129,13 +2221,13 @@
         <v>56</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>317</v>
+        <v>496</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2143,13 +2235,13 @@
         <v>52</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>309</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2157,13 +2249,13 @@
         <v>62</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>310</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2177,7 +2269,7 @@
         <v>311</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2185,13 +2277,13 @@
         <v>58</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>312</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2199,13 +2291,13 @@
         <v>59</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>313</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2219,7 +2311,7 @@
         <v>314</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2233,7 +2325,7 @@
         <v>315</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2247,7 +2339,7 @@
         <v>316</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2258,10 +2350,10 @@
         <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2272,13 +2364,13 @@
         <v>11</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
         <v>14</v>
       </c>
@@ -2286,10 +2378,10 @@
         <v>15</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2353,13 +2445,13 @@
         <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2370,10 +2462,10 @@
         <v>26</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -2384,10 +2476,10 @@
         <v>28</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -2398,10 +2490,10 @@
         <v>30</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2412,10 +2504,10 @@
         <v>32</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -2426,10 +2518,10 @@
         <v>34</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -2437,13 +2529,13 @@
         <v>35</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -2454,10 +2546,10 @@
         <v>76</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -2468,10 +2560,10 @@
         <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -2482,10 +2574,10 @@
         <v>39</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -2496,10 +2588,10 @@
         <v>41</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -2510,10 +2602,10 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D40" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -2527,7 +2619,7 @@
         <v>43</v>
       </c>
       <c r="D41" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -2538,10 +2630,10 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -2552,7 +2644,7 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -2563,13 +2655,13 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D44" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -2580,10 +2672,10 @@
         <v>67</v>
       </c>
       <c r="C45" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D45" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -2594,10 +2686,10 @@
         <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D46" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -2608,10 +2700,10 @@
         <v>71</v>
       </c>
       <c r="C47" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D47" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -2622,10 +2714,10 @@
         <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D48" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -2633,13 +2725,13 @@
         <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C49" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D49" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -2647,13 +2739,13 @@
         <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C50" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D50" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -2661,41 +2753,41 @@
         <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C51" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D51" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B52" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C52" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D52" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B53" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C53" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D53" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2706,10 +2798,10 @@
         <v>80</v>
       </c>
       <c r="C54" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -2723,7 +2815,7 @@
         <v>81</v>
       </c>
       <c r="D55" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2734,10 +2826,10 @@
         <v>82</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D56" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -2748,10 +2840,10 @@
         <v>98</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -2762,10 +2854,10 @@
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2776,10 +2868,10 @@
         <v>99</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2790,10 +2882,10 @@
         <v>96</v>
       </c>
       <c r="C60" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2804,38 +2896,38 @@
         <v>97</v>
       </c>
       <c r="C61" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B63" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C63" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2846,10 +2938,10 @@
         <v>90</v>
       </c>
       <c r="C64" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2860,10 +2952,10 @@
         <v>92</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2874,10 +2966,10 @@
         <v>94</v>
       </c>
       <c r="C66" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2888,10 +2980,10 @@
         <v>95</v>
       </c>
       <c r="C67" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2902,10 +2994,10 @@
         <v>101</v>
       </c>
       <c r="C68" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2916,10 +3008,10 @@
         <v>104</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2930,10 +3022,10 @@
         <v>103</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2944,10 +3036,10 @@
         <v>102</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2958,10 +3050,10 @@
         <v>110</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2972,10 +3064,10 @@
         <v>109</v>
       </c>
       <c r="C73" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D73" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2986,10 +3078,10 @@
         <v>112</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -3000,10 +3092,10 @@
         <v>114</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -3014,10 +3106,10 @@
         <v>116</v>
       </c>
       <c r="C76" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D76" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -3031,7 +3123,7 @@
         <v>316</v>
       </c>
       <c r="D77" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -3039,13 +3131,13 @@
         <v>118</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -3056,10 +3148,10 @@
         <v>119</v>
       </c>
       <c r="C79" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D79" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -3070,10 +3162,10 @@
         <v>121</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -3081,13 +3173,13 @@
         <v>123</v>
       </c>
       <c r="B81" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C81" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D81" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -3095,969 +3187,913 @@
         <v>124</v>
       </c>
       <c r="B82" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C82" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D82" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B87" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B87" s="19" t="s">
-        <v>283</v>
-      </c>
       <c r="C87" s="19" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B88" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D88" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B89" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D89" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B90" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D90" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B91" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D91" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>383</v>
+        <v>498</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B96" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C96" t="s">
-        <v>382</v>
+        <v>499</v>
       </c>
       <c r="D96" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B97" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C97" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D97" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B98" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C98" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D98" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B99" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C99" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D99" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B100" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C100" t="s">
-        <v>388</v>
+        <v>475</v>
       </c>
       <c r="D100" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B101" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C101" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D101" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B102" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C102" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D102" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B103" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C103" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D103" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B104" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C104" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D104" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B105" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C105" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D105" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>186</v>
+      </c>
+      <c r="B106" t="s">
         <v>185</v>
       </c>
-      <c r="B106" t="s">
-        <v>184</v>
-      </c>
       <c r="C106" t="s">
-        <v>394</v>
+        <v>494</v>
       </c>
       <c r="D106" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B107" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="C107" t="s">
-        <v>396</v>
+        <v>458</v>
       </c>
       <c r="D107" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="B108" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C108" t="s">
-        <v>397</v>
+        <v>459</v>
       </c>
       <c r="D108" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B109" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="C109" t="s">
-        <v>399</v>
+        <v>495</v>
       </c>
       <c r="D109" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B110" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C110" t="s">
-        <v>402</v>
+        <v>460</v>
       </c>
       <c r="D110" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B111" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C111" t="s">
-        <v>404</v>
+        <v>461</v>
       </c>
       <c r="D111" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B112" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C112" t="s">
-        <v>406</v>
+        <v>462</v>
       </c>
       <c r="D112" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B113" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C113" t="s">
-        <v>407</v>
+        <v>463</v>
       </c>
       <c r="D113" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B114" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C114" t="s">
-        <v>409</v>
+        <v>465</v>
       </c>
       <c r="D114" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B115" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C115" t="s">
-        <v>411</v>
+        <v>464</v>
       </c>
       <c r="D115" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B116" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C116" t="s">
-        <v>412</v>
+        <v>329</v>
       </c>
       <c r="D116" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B117" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C117" t="s">
-        <v>413</v>
+        <v>466</v>
       </c>
       <c r="D117" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="C118" s="11" t="s">
-        <v>415</v>
+        <v>411</v>
+      </c>
+      <c r="C118" t="s">
+        <v>467</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B119" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C119" t="s">
-        <v>416</v>
+        <v>468</v>
       </c>
       <c r="D119" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B120" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C120" t="s">
-        <v>418</v>
+        <v>469</v>
       </c>
       <c r="D120" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B121" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C121" t="s">
-        <v>419</v>
+        <v>470</v>
       </c>
       <c r="D121" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="20" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B122" s="20" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C122" s="20" t="s">
-        <v>422</v>
+        <v>471</v>
       </c>
       <c r="D122" s="20" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="20" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B123" s="20" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C123" s="20" t="s">
-        <v>423</v>
+        <v>497</v>
       </c>
       <c r="D123" s="20" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="20" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B124" s="20" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C124" s="20" t="s">
-        <v>427</v>
+        <v>472</v>
       </c>
       <c r="D124" s="20" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="20" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B125" s="20" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C125" s="20" t="s">
-        <v>428</v>
+        <v>473</v>
       </c>
       <c r="D125" s="20" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="20" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B126" s="20" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C126" s="20" t="s">
-        <v>430</v>
+        <v>474</v>
       </c>
       <c r="D126" s="20" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="20" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B127" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C127" s="20" t="s">
-        <v>432</v>
+        <v>476</v>
       </c>
       <c r="D127" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="20" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B128" s="20" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>434</v>
+        <v>477</v>
       </c>
       <c r="D128" s="20" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="20" t="s">
-        <v>435</v>
+        <v>93</v>
       </c>
       <c r="B129" s="20" t="s">
-        <v>436</v>
+        <v>126</v>
       </c>
       <c r="C129" s="20" t="s">
-        <v>436</v>
+        <v>371</v>
       </c>
       <c r="D129" s="20" t="s">
-        <v>436</v>
+        <v>126</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="20" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="B130" s="20" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C130" s="20" t="s">
-        <v>437</v>
+        <v>493</v>
       </c>
       <c r="D130" s="20" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="20" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B131" s="20" t="s">
-        <v>103</v>
+        <v>434</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>103</v>
+        <v>358</v>
       </c>
       <c r="D131" s="20" t="s">
-        <v>103</v>
+        <v>434</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="20" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B132" s="20" t="s">
-        <v>441</v>
+        <v>103</v>
       </c>
       <c r="C132" s="20" t="s">
-        <v>441</v>
+        <v>478</v>
       </c>
       <c r="D132" s="20" t="s">
-        <v>441</v>
+        <v>103</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="20" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C133" s="20" t="s">
-        <v>443</v>
+        <v>479</v>
       </c>
       <c r="D133" s="20" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="20" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="B134" s="20" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C134" s="20" t="s">
-        <v>444</v>
+        <v>480</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="20" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B135" s="20" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="C135" s="20" t="s">
-        <v>447</v>
+        <v>481</v>
       </c>
       <c r="D135" s="20" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="20" t="s">
-        <v>448</v>
-      </c>
-      <c r="B136" s="20" t="s">
-        <v>449</v>
+        <v>443</v>
+      </c>
+      <c r="B136" s="27" t="s">
+        <v>482</v>
       </c>
       <c r="C136" s="20" t="s">
-        <v>449</v>
-      </c>
-      <c r="D136" s="20" t="s">
-        <v>449</v>
+        <v>483</v>
+      </c>
+      <c r="D136" s="27" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="20" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="B137" s="20" t="s">
-        <v>92</v>
+        <v>445</v>
       </c>
       <c r="C137" s="20" t="s">
-        <v>92</v>
+        <v>352</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>92</v>
+        <v>445</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="20" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>95</v>
+        <v>485</v>
       </c>
       <c r="D138" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="20" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="B139" s="20" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="C139" s="20" t="s">
-        <v>140</v>
+        <v>484</v>
       </c>
       <c r="D139" s="20" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="20" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="B140" s="20" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C140" s="20" t="s">
-        <v>138</v>
+        <v>486</v>
       </c>
       <c r="D140" s="20" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="20" t="s">
-        <v>93</v>
+        <v>449</v>
       </c>
       <c r="B141" s="20" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="C141" s="20" t="s">
-        <v>94</v>
+        <v>487</v>
       </c>
       <c r="D141" s="20" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="20" t="s">
-        <v>454</v>
+        <v>93</v>
       </c>
       <c r="B142" s="20" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C142" s="20" t="s">
-        <v>92</v>
+        <v>488</v>
       </c>
       <c r="D142" s="20" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="20" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="B143" s="20" t="s">
-        <v>455</v>
+        <v>92</v>
       </c>
       <c r="C143" s="20" t="s">
-        <v>455</v>
+        <v>489</v>
       </c>
       <c r="D143" s="20" t="s">
-        <v>455</v>
+        <v>92</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="20" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="B144" s="20" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="C144" s="20" t="s">
-        <v>457</v>
+        <v>490</v>
       </c>
       <c r="D144" s="20" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="20" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B145" s="20" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="C145" s="20" t="s">
-        <v>460</v>
+        <v>491</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A146" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A147" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A148" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D148" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A149" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="D149" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A150" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="B150" s="21" t="s">
-        <v>283</v>
-      </c>
-      <c r="C150" s="21" t="s">
-        <v>283</v>
-      </c>
-      <c r="D150" s="21" t="s">
-        <v>283</v>
+      <c r="A146" s="20" t="s">
+        <v>455</v>
+      </c>
+      <c r="B146" s="20" t="s">
+        <v>456</v>
+      </c>
+      <c r="C146" s="20" t="s">
+        <v>492</v>
+      </c>
+      <c r="D146" s="20" t="s">
+        <v>456</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D135" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}"/>
+  <autoFilter ref="A1:D136" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New SNR options and a playful volume meter
</commit_message>
<xml_diff>
--- a/data-raw/musicassessr_dict.xlsx
+++ b/data-raw/musicassessr_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C3AC44-61A3-9640-AE92-2BDB9A7AB63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD97BFDA-9409-C841-81EA-9EAB1E7F75B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="3960" windowWidth="35840" windowHeight="20720" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="35840" windowHeight="20720" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="530">
   <si>
     <t>mar_can_hear</t>
   </si>
@@ -579,9 +579,6 @@
     <t>long_tone_text</t>
   </si>
   <si>
-    <t>Sing along with the tone for 5 seconds.</t>
-  </si>
-  <si>
     <t>you_have_completed_the</t>
   </si>
   <si>
@@ -810,9 +807,6 @@
     <t>Singen Sie mit diesem Ton mit.</t>
   </si>
   <si>
-    <t>Singen Sie 5 Sekunden lang mit dem Tom mit.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mikrofon </t>
   </si>
   <si>
@@ -1566,9 +1560,6 @@
     <t>long_tone_text_call_and_response</t>
   </si>
   <si>
-    <t>Sing this note for 5 seconds after you hear it.</t>
-  </si>
-  <si>
     <t>long_tone_instruction_call_and_response</t>
   </si>
   <si>
@@ -1606,13 +1597,43 @@
   </si>
   <si>
     <t>Per favore, inserisci il tuo codice.</t>
+  </si>
+  <si>
+    <t>Sing this note for several seconds after you hear it.</t>
+  </si>
+  <si>
+    <t>Sing along with the tone for several seconds.</t>
+  </si>
+  <si>
+    <t>Singen Sie mehrere Sekunden lang mit dem Tom mit.</t>
+  </si>
+  <si>
+    <t>sure_continue</t>
+  </si>
+  <si>
+    <t>Are you sure you want to continue?</t>
+  </si>
+  <si>
+    <t>Continue_Anyway</t>
+  </si>
+  <si>
+    <t>Continue Anyway</t>
+  </si>
+  <si>
+    <t>Weitermachen Trotzdem</t>
+  </si>
+  <si>
+    <t>record_instructions_playful</t>
+  </si>
+  <si>
+    <t>When you sing, you will see a bird appear. Try testing this now by singing and watching the bird appear.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1633,13 +1654,32 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -1674,7 +1714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1696,6 +1736,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2010,10 +2060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}">
-  <dimension ref="A1:D154"/>
+  <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2033,7 +2083,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>126</v>
@@ -2047,10 +2097,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2061,10 +2111,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2072,13 +2122,13 @@
         <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2086,13 +2136,13 @@
         <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2103,24 +2153,24 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>277</v>
+        <v>298</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2128,13 +2178,13 @@
         <v>51</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2145,24 +2195,24 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>280</v>
+        <v>302</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2173,10 +2223,10 @@
         <v>57</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2184,13 +2234,13 @@
         <v>54</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2198,13 +2248,13 @@
         <v>56</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2215,10 +2265,10 @@
         <v>178</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2226,13 +2276,13 @@
         <v>62</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2243,10 +2293,10 @@
         <v>64</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2257,10 +2307,10 @@
         <v>128</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2271,10 +2321,10 @@
         <v>129</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2285,10 +2335,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2299,10 +2349,10 @@
         <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2313,10 +2363,10 @@
         <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2327,10 +2377,10 @@
         <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2341,10 +2391,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2355,10 +2405,10 @@
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2425,10 +2475,10 @@
         <v>131</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2439,10 +2489,10 @@
         <v>26</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -2453,10 +2503,10 @@
         <v>28</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -2467,10 +2517,10 @@
         <v>30</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2481,10 +2531,10 @@
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -2495,10 +2545,10 @@
         <v>34</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -2506,13 +2556,13 @@
         <v>35</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -2523,10 +2573,10 @@
         <v>76</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -2537,10 +2587,10 @@
         <v>37</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -2551,10 +2601,10 @@
         <v>39</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -2565,10 +2615,10 @@
         <v>41</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -2579,7 +2629,7 @@
         <v>42</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>140</v>
@@ -2607,7 +2657,7 @@
         <v>44</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>142</v>
@@ -2621,7 +2671,7 @@
         <v>45</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>45</v>
@@ -2635,10 +2685,10 @@
         <v>130</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -2649,10 +2699,10 @@
         <v>67</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -2663,10 +2713,10 @@
         <v>69</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -2677,10 +2727,10 @@
         <v>71</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -2691,10 +2741,10 @@
         <v>73</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -2702,13 +2752,13 @@
         <v>74</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -2719,10 +2769,10 @@
         <v>158</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -2733,10 +2783,10 @@
         <v>159</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -2747,10 +2797,10 @@
         <v>160</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -2761,10 +2811,10 @@
         <v>161</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2775,10 +2825,10 @@
         <v>80</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -2792,7 +2842,7 @@
         <v>81</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2803,10 +2853,10 @@
         <v>82</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -2817,10 +2867,10 @@
         <v>98</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -2831,10 +2881,10 @@
         <v>7</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2845,10 +2895,10 @@
         <v>99</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2859,10 +2909,10 @@
         <v>96</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2873,10 +2923,10 @@
         <v>97</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2887,10 +2937,10 @@
         <v>137</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2901,10 +2951,10 @@
         <v>139</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2915,10 +2965,10 @@
         <v>90</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2929,10 +2979,10 @@
         <v>92</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2943,10 +2993,10 @@
         <v>94</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2957,10 +3007,10 @@
         <v>95</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2971,10 +3021,10 @@
         <v>101</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2985,10 +3035,10 @@
         <v>104</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2999,10 +3049,10 @@
         <v>103</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -3013,10 +3063,10 @@
         <v>102</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -3027,10 +3077,10 @@
         <v>110</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -3041,10 +3091,10 @@
         <v>109</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -3052,13 +3102,13 @@
         <v>111</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -3069,10 +3119,10 @@
         <v>113</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -3083,10 +3133,10 @@
         <v>115</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -3097,10 +3147,10 @@
         <v>116</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -3108,13 +3158,13 @@
         <v>117</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -3125,10 +3175,10 @@
         <v>118</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -3139,10 +3189,10 @@
         <v>120</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -3150,13 +3200,13 @@
         <v>122</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -3164,27 +3214,27 @@
         <v>123</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -3192,55 +3242,55 @@
         <v>179</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>180</v>
+        <v>521</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>257</v>
+        <v>522</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -3251,10 +3301,10 @@
         <v>125</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -3279,10 +3329,10 @@
         <v>133</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -3293,7 +3343,7 @@
         <v>135</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>143</v>
@@ -3307,7 +3357,7 @@
         <v>145</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>146</v>
@@ -3321,10 +3371,10 @@
         <v>148</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -3335,7 +3385,7 @@
         <v>150</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>151</v>
@@ -3349,10 +3399,10 @@
         <v>153</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -3363,10 +3413,10 @@
         <v>155</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -3377,10 +3427,10 @@
         <v>163</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -3391,10 +3441,10 @@
         <v>166</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -3405,10 +3455,10 @@
         <v>167</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -3419,10 +3469,10 @@
         <v>170</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -3433,10 +3483,10 @@
         <v>169</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -3447,10 +3497,10 @@
         <v>173</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -3461,10 +3511,10 @@
         <v>175</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -3475,513 +3525,513 @@
         <v>177</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B105" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="C105" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>388</v>
+        <v>453</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>389</v>
+        <v>454</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>391</v>
+        <v>490</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D110" s="12" t="s">
         <v>393</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>397</v>
+        <v>456</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>399</v>
+        <v>457</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>400</v>
+        <v>458</v>
+      </c>
+      <c r="D113" s="12" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>402</v>
+        <v>460</v>
+      </c>
+      <c r="D114" s="12" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>404</v>
+        <v>459</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>405</v>
+        <v>325</v>
+      </c>
+      <c r="D116" s="12" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>409</v>
+        <v>461</v>
+      </c>
+      <c r="D117" s="12" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D118" s="9" t="s">
-        <v>408</v>
+        <v>462</v>
+      </c>
+      <c r="D118" s="13" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>410</v>
+        <v>463</v>
+      </c>
+      <c r="D119" s="12" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>412</v>
+        <v>464</v>
+      </c>
+      <c r="D120" s="12" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>413</v>
+        <v>465</v>
+      </c>
+      <c r="D121" s="12" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>416</v>
+        <v>466</v>
+      </c>
+      <c r="D122" s="12" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>417</v>
+        <v>492</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>421</v>
+        <v>467</v>
+      </c>
+      <c r="D124" s="12" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>422</v>
+        <v>468</v>
+      </c>
+      <c r="D125" s="12" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>424</v>
+        <v>469</v>
+      </c>
+      <c r="D126" s="12" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>426</v>
+        <v>471</v>
+      </c>
+      <c r="D127" s="12" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>428</v>
+        <v>472</v>
+      </c>
+      <c r="D128" s="12" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>430</v>
+        <v>488</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>431</v>
+        <v>354</v>
+      </c>
+      <c r="D130" s="12" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="D131" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D131" s="12" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>435</v>
+        <v>474</v>
+      </c>
+      <c r="D132" s="12" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>437</v>
+        <v>475</v>
+      </c>
+      <c r="D133" s="12" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>438</v>
+        <v>476</v>
+      </c>
+      <c r="D134" s="12" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="D135" s="10" t="s">
-        <v>479</v>
+        <v>478</v>
+      </c>
+      <c r="D135" s="14" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>442</v>
+        <v>348</v>
+      </c>
+      <c r="D136" s="12" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="D137" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="D137" s="12" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="D138" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="D138" s="12" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>139</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="D139" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="D139" s="12" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="D140" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="D140" s="12" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3993,192 +4043,234 @@
         <v>94</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="D141" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="D141" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="D142" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="D142" s="12" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>448</v>
+        <v>485</v>
+      </c>
+      <c r="D143" s="12" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>450</v>
+        <v>486</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>453</v>
+        <v>487</v>
+      </c>
+      <c r="D145" s="12" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>499</v>
+        <v>513</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>501</v>
+        <v>514</v>
+      </c>
+      <c r="D147" s="12" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="D148" s="2" t="s">
-        <v>503</v>
+        <v>515</v>
+      </c>
+      <c r="D148" s="12" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="D149" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
+      </c>
+      <c r="D149" s="12" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>509</v>
+        <v>520</v>
+      </c>
+      <c r="D150" s="12" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="B151" s="2" t="s">
-        <v>513</v>
-      </c>
       <c r="C151" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="D151" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
+      </c>
+      <c r="D151" s="12" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="B152" s="2" t="s">
-        <v>514</v>
-      </c>
       <c r="C152" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="D152" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
+      </c>
+      <c r="D152" s="12" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B153" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="B153" s="3" t="s">
-        <v>515</v>
-      </c>
       <c r="C153" s="3" t="s">
-        <v>515</v>
-      </c>
-      <c r="D153" s="3" t="s">
-        <v>515</v>
+        <v>512</v>
+      </c>
+      <c r="D153" s="11" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C154" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="B154" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>522</v>
-      </c>
       <c r="D154" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B155" s="16" t="s">
+        <v>524</v>
+      </c>
+      <c r="C155" s="16" t="s">
+        <v>524</v>
+      </c>
+      <c r="D155" s="16" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" s="15" t="s">
+        <v>525</v>
+      </c>
+      <c r="B156" s="15" t="s">
+        <v>526</v>
+      </c>
+      <c r="C156" s="15" t="s">
+        <v>526</v>
+      </c>
+      <c r="D156" s="15" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Async feedback and lyric features
</commit_message>
<xml_diff>
--- a/data-raw/musicassessr_dict.xlsx
+++ b/data-raw/musicassessr_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4481F2F1-4E9C-FE45-B3DF-52F202C764DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CC52B7-257A-694F-BDDF-C22F483F3C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="746">
   <si>
     <t>mar_can_hear</t>
   </si>
@@ -2294,13 +2294,10 @@
     <t xml:space="preserve">Thank you! You have completed the </t>
   </si>
   <si>
-    <t>the_lyrics_are</t>
-  </si>
-  <si>
-    <t>The lyrics are:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Der Text lautet: </t>
+    <t>Lyrics</t>
+  </si>
+  <si>
+    <t>Songtext</t>
   </si>
 </sst>
 </file>
@@ -2743,8 +2740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}">
   <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D173" sqref="D173"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5583,16 +5580,16 @@
         <v>744</v>
       </c>
       <c r="B167" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="D167" s="2" t="s">
         <v>745</v>
       </c>
-      <c r="C167" s="2" t="s">
-        <v>745</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>746</v>
-      </c>
       <c r="E167" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commits to support SongBird
</commit_message>
<xml_diff>
--- a/data-raw/musicassessr_dict.xlsx
+++ b/data-raw/musicassessr_dict.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E540A2B-2E95-444B-AEC0-CB31C5E6930F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3556E866-3EF7-274A-80DC-52D01C6FDC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="35840" windowHeight="20720" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$D$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$E$180</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="792">
   <si>
     <t>mar_can_hear</t>
   </si>
@@ -2371,9 +2371,6 @@
     <t>Singe die Melodie nach.</t>
   </si>
   <si>
-    <t>lets_proceed</t>
-  </si>
-  <si>
     <t>Let's proceed!</t>
   </si>
   <si>
@@ -2423,13 +2420,32 @@
   </si>
   <si>
     <t>Now_you_will_hear_some</t>
+  </si>
+  <si>
+    <t>continue_learning_question</t>
+  </si>
+  <si>
+    <t>Would you like to continue learning? </t>
+  </si>
+  <si>
+    <t>Mochten Sie weiterlernen?</t>
+  </si>
+  <si>
+    <t>redirect_message2</t>
+  </si>
+  <si>
+    <t>Thank you! You will now be redirected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danke! Sie werden jetzt zurückgeleitet.
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2478,6 +2494,12 @@
       <charset val="186"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2519,7 +2541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2552,6 +2574,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2866,10 +2889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A179" sqref="A179"/>
+    <sheetView tabSelected="1" topLeftCell="C157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5807,124 +5830,159 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>769</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="C173" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="D173" t="s">
         <v>770</v>
       </c>
-      <c r="C173" s="2" t="s">
-        <v>770</v>
-      </c>
-      <c r="D173" t="s">
-        <v>771</v>
-      </c>
       <c r="E173" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>772</v>
       </c>
-      <c r="B174" s="2" t="s">
-        <v>773</v>
-      </c>
       <c r="C174" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A180" s="2" t="s">
         <v>786</v>
       </c>
-      <c r="B179" s="2" t="s">
-        <v>779</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>779</v>
-      </c>
-      <c r="D179" s="2" t="s">
-        <v>785</v>
-      </c>
-      <c r="E179" s="2" t="s">
-        <v>779</v>
+      <c r="B180" s="16" t="s">
+        <v>787</v>
+      </c>
+      <c r="C180" s="16" t="s">
+        <v>787</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="E180" s="16" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A181" s="12" t="s">
+        <v>789</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="D181" s="15" t="s">
+        <v>791</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>790</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E180" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New selected item bank and features
</commit_message>
<xml_diff>
--- a/data-raw/musicassessr_dict.xlsx
+++ b/data-raw/musicassessr_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEB6C57-D8B6-E046-BF02-8FF5D3AFDF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1878DE26-44B9-6742-B515-40301CE339A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1700" windowWidth="35840" windowHeight="20700" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20700" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="1010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="1009">
   <si>
     <t>mar_can_hear</t>
   </si>
@@ -3051,9 +3051,6 @@
   </si>
   <si>
     <t>Singen</t>
-  </si>
-  <si>
-    <t>Singe</t>
   </si>
   <si>
     <t>play_the_melody</t>
@@ -3541,8 +3538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}">
   <dimension ref="A1:E258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="B205" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B212" sqref="B212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4100,16 +4097,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>1007</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>1008</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>1008</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>1009</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>905</v>
@@ -4576,16 +4573,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>1004</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>1005</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>905</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>905</v>
@@ -5137,16 +5134,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>905</v>
       </c>
       <c r="D94" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>905</v>
@@ -6378,16 +6375,16 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="C167" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="D167" s="1" t="s">
         <v>999</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>999</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>1000</v>
       </c>
       <c r="E167" s="5"/>
     </row>
@@ -7144,7 +7141,7 @@
         <v>995</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>905</v>
@@ -7161,7 +7158,7 @@
         <v>880</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>918</v>
+        <v>880</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>905</v>

</xml_diff>